<commit_message>
Add Central App Router to MultiServerMultiAuth sample app
</commit_message>
<xml_diff>
--- a/MultiServerAuth-MultiRoutingAuth/Roles and scopes mapping.xlsx
+++ b/MultiServerAuth-MultiRoutingAuth/Roles and scopes mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/I537744/dev/SAP/SAP_CFSamples/MultiServerAuth-MultiRoutingAuth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53735B8-29F6-054E-BBE4-51B79931E0E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDD3382-2D73-5044-BCB8-E388EF665766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25980" yWindow="620" windowWidth="21560" windowHeight="26580" xr2:uid="{0C78704F-321F-2E41-ACCC-58116A9301CF}"/>
+    <workbookView xWindow="25980" yWindow="500" windowWidth="21560" windowHeight="26600" xr2:uid="{0C78704F-321F-2E41-ACCC-58116A9301CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -175,25 +175,25 @@
     <t>two_api_admin</t>
   </si>
   <si>
-    <t>two_admin</t>
-  </si>
-  <si>
     <t>TWO Admin</t>
   </si>
   <si>
     <t>ONE Admin</t>
   </si>
   <si>
-    <t>one_admin</t>
-  </si>
-  <si>
-    <t>basic_user</t>
-  </si>
-  <si>
     <t>one_api_basic_editor</t>
   </si>
   <si>
     <t>two_api_basic_reader</t>
+  </si>
+  <si>
+    <t>multiauth_basic_user</t>
+  </si>
+  <si>
+    <t>multiauth_one_admin</t>
+  </si>
+  <si>
+    <t>multiauth_two_admin</t>
   </si>
 </sst>
 </file>
@@ -1661,7 +1661,7 @@
   <dimension ref="B3:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:E9"/>
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1922,7 +1922,7 @@
       <c r="D22" s="33"/>
       <c r="E22" s="34"/>
       <c r="F22" s="35" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G22" s="11" t="s">
         <v>7</v>
@@ -1990,7 +1990,7 @@
         <v>31</v>
       </c>
       <c r="F28" s="43" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G28" s="44" t="s">
         <v>7</v>
@@ -2212,10 +2212,10 @@
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="58" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E47" s="59" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F47" s="72" t="s">
         <v>39</v>
@@ -2240,10 +2240,10 @@
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="75" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E49" s="75" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="F49" s="76" t="s">
         <v>45</v>

</xml_diff>